<commit_message>
fixed typos in part numbers
</commit_message>
<xml_diff>
--- a/Part nr. full assembled smfScope up to date.xlsx
+++ b/Part nr. full assembled smfScope up to date.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Excitation path" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="200">
   <si>
     <t>Part Nr.</t>
   </si>
@@ -196,9 +196,6 @@
     <t>RS10/M</t>
   </si>
   <si>
-    <t>TR50/M0</t>
-  </si>
-  <si>
     <t>Pedestal Pillar Post BS1 (L=1'')</t>
   </si>
   <si>
@@ -253,12 +250,6 @@
     <t>2x4 Rod adapter BS1 to box</t>
   </si>
   <si>
-    <t>DC1-DCH/M</t>
-  </si>
-  <si>
-    <t>UPH/30/M</t>
-  </si>
-  <si>
     <t>NC395323-T640lpxr</t>
   </si>
   <si>
@@ -271,9 +262,6 @@
     <t>AC254-75-B-ML</t>
   </si>
   <si>
-    <t>SML03</t>
-  </si>
-  <si>
     <t>APD0 (Excelitas)</t>
   </si>
   <si>
@@ -364,9 +352,6 @@
     <t>CXYZ05/M</t>
   </si>
   <si>
-    <t>CWY1</t>
-  </si>
-  <si>
     <t>Translating Lens Mount for L4</t>
   </si>
   <si>
@@ -403,12 +388,6 @@
     <t>FOC bushing adapter (Ext. SM1 Int. M25)</t>
   </si>
   <si>
-    <t>SH4S038</t>
-  </si>
-  <si>
-    <t>Screws for DC1</t>
-  </si>
-  <si>
     <t>M3</t>
   </si>
   <si>
@@ -418,24 +397,15 @@
     <t>Nanostage Z</t>
   </si>
   <si>
-    <t>LT2.100</t>
-  </si>
-  <si>
     <t>LightHUB-2</t>
   </si>
   <si>
     <t>Laser (515nm 80 mW, 638nm 100mW)</t>
   </si>
   <si>
-    <t>Screws?</t>
-  </si>
-  <si>
     <t>Lens Tube L4 (0.5'')</t>
   </si>
   <si>
-    <t>Nanostage XY (Not used)</t>
-  </si>
-  <si>
     <t>AC254-030-AML</t>
   </si>
   <si>
@@ -653,6 +623,9 @@
   </si>
   <si>
     <t>Precision mount for DM1</t>
+  </si>
+  <si>
+    <t>UPH30/M</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1143,7 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="A3" sqref="A3:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,10 +1159,10 @@
   <sheetData>
     <row r="1" spans="1:11" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>0</v>
@@ -1200,24 +1173,24 @@
     </row>
     <row r="2" spans="1:11" ht="24" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="7" customFormat="1" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="F3" s="20" t="s">
         <v>22</v>
@@ -1231,7 +1204,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D4" s="26">
         <v>27</v>
@@ -1240,7 +1213,7 @@
         <v>55</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1251,7 +1224,7 @@
         <v>29</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="D5" s="26">
         <v>28</v>
@@ -1271,7 +1244,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D6" s="26">
         <v>29</v>
@@ -1280,7 +1253,7 @@
         <v>54</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1300,7 +1273,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1320,7 +1293,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1328,7 +1301,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>33</v>
@@ -1337,10 +1310,10 @@
         <v>32</v>
       </c>
       <c r="E9" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="27" t="s">
         <v>64</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1360,7 +1333,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1377,10 +1350,10 @@
         <v>34</v>
       </c>
       <c r="E11" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="27" t="s">
         <v>67</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1400,7 +1373,7 @@
         <v>24</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1420,7 +1393,7 @@
         <v>15</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1440,7 +1413,7 @@
         <v>16</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1460,7 +1433,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1477,10 +1450,10 @@
         <v>39</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1500,7 +1473,7 @@
         <v>15</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1520,7 +1493,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1540,7 +1513,7 @@
         <v>25</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1548,7 +1521,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>47</v>
@@ -1560,7 +1533,7 @@
         <v>23</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1580,7 +1553,7 @@
         <v>29</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1597,10 +1570,10 @@
         <v>45</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1617,10 +1590,10 @@
         <v>46</v>
       </c>
       <c r="E23" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="27" t="s">
         <v>70</v>
-      </c>
-      <c r="F23" s="27" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1640,7 +1613,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1660,7 +1633,7 @@
         <v>30</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1668,7 +1641,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" s="25" t="s">
         <v>50</v>
@@ -1680,7 +1653,7 @@
         <v>30</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1691,16 +1664,16 @@
         <v>9</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="E27" s="30">
         <v>21012</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1714,13 +1687,13 @@
         <v>53</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1728,19 +1701,19 @@
         <v>26</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" s="30">
         <v>49793</v>
       </c>
       <c r="F29" s="29" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1823,10 +1796,10 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C59" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1843,10 +1816,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F31"/>
+  <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,24 +1834,24 @@
   <sheetData>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="11" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="F3" s="32" t="s">
         <v>22</v>
@@ -1889,10 +1862,10 @@
         <v>48</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="D4" s="34">
         <v>59</v>
@@ -1901,7 +1874,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1909,19 +1882,19 @@
         <v>49</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D5" s="34">
         <v>60</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>112</v>
+        <v>2</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1929,19 +1902,19 @@
         <v>50</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D6" s="34">
         <v>61</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1949,19 +1922,19 @@
         <v>51</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="D7" s="34">
         <v>62</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1969,19 +1942,19 @@
         <v>52</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D8" s="34">
         <v>63</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1989,19 +1962,19 @@
         <v>53</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="D9" s="34">
         <v>64</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2012,7 +1985,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="D10" s="34">
         <v>65</v>
@@ -2021,7 +1994,7 @@
         <v>14</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2029,19 +2002,19 @@
         <v>55</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2049,19 +2022,19 @@
         <v>56</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2069,19 +2042,19 @@
         <v>57</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E13" s="39">
         <v>49792</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2089,19 +2062,19 @@
         <v>58</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2141,27 +2114,6 @@
       <c r="A25" s="15"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>125</v>
-      </c>
-      <c r="C29" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>130</v>
-      </c>
-      <c r="C31" t="s">
-        <v>135</v>
-      </c>
     </row>
   </sheetData>
   <sortState ref="A5:C30">
@@ -2176,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,29 +2144,29 @@
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="F3" s="20" t="s">
         <v>22</v>
@@ -2228,7 +2180,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="D4" s="23">
         <v>86</v>
@@ -2237,7 +2189,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2248,7 +2200,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="D5" s="23">
         <v>87</v>
@@ -2257,7 +2209,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2268,7 +2220,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="D6" s="23">
         <v>88</v>
@@ -2277,7 +2229,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2288,7 +2240,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="D7" s="23">
         <v>89</v>
@@ -2297,7 +2249,7 @@
         <v>44</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2308,7 +2260,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D8" s="23">
         <v>90</v>
@@ -2317,7 +2269,7 @@
         <v>11</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2328,7 +2280,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="D9" s="23">
         <v>91</v>
@@ -2337,7 +2289,7 @@
         <v>7</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2345,10 +2297,10 @@
         <v>72</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D10" s="23">
         <v>92</v>
@@ -2357,7 +2309,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2368,7 +2320,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="D11" s="23">
         <v>93</v>
@@ -2377,7 +2329,7 @@
         <v>18</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2388,7 +2340,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D12" s="23">
         <v>94</v>
@@ -2397,7 +2349,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="40" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2405,19 +2357,19 @@
         <v>75</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>76</v>
+        <v>199</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="D13" s="23">
         <v>95</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>81</v>
+        <v>15</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2428,7 +2380,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="D14" s="23">
         <v>96</v>
@@ -2437,7 +2389,7 @@
         <v>6</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2448,16 +2400,16 @@
         <v>18</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="D15" s="23">
         <v>97</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2468,7 +2420,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="D16" s="23">
         <v>98</v>
@@ -2477,7 +2429,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2485,19 +2437,19 @@
         <v>79</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>81</v>
+        <v>15</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="D17" s="23">
         <v>99</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2508,16 +2460,16 @@
         <v>6</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E18" s="30">
         <v>49793</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2525,19 +2477,19 @@
         <v>81</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2548,16 +2500,16 @@
         <v>1</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E20" s="29" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="29" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2565,19 +2517,19 @@
         <v>83</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D21" s="42" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F21" s="29" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2585,19 +2537,19 @@
         <v>84</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="D22" s="42" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2608,16 +2560,16 @@
         <v>4</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2702,7 +2654,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>